<commit_message>
Updated work time and R2
</commit_message>
<xml_diff>
--- a/Reports/Time_Worked.xlsx
+++ b/Reports/Time_Worked.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
   <si>
     <t>Documentation</t>
   </si>
@@ -60,16 +60,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>UML</t>
-  </si>
-  <si>
-    <t>0.5</t>
-  </si>
-  <si>
-    <t>1.5</t>
   </si>
 </sst>
 </file>
@@ -111,13 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -420,7 +408,7 @@
   <dimension ref="A1:F39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -456,17 +444,21 @@
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>16</v>
+      <c r="B3" s="2">
+        <v>3</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
@@ -476,45 +468,57 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>3</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
+      <c r="B5" s="2">
+        <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>3</v>
-      </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1">
-        <v>0</v>
+      <c r="B6" s="2">
+        <v>3</v>
       </c>
       <c r="C6" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
@@ -529,8 +533,12 @@
       <c r="D7" s="1">
         <v>0</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="C9" t="s">
@@ -558,17 +566,21 @@
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -577,14 +589,18 @@
       <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="1">
         <v>0</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
@@ -593,14 +609,18 @@
       <c r="B13">
         <v>0</v>
       </c>
-      <c r="C13" s="4">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -609,14 +629,18 @@
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>0</v>
       </c>
       <c r="D14" s="1">
         <v>0</v>
       </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
@@ -625,14 +649,18 @@
       <c r="B15">
         <v>0</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="C17" t="s">
@@ -663,17 +691,17 @@
       <c r="B19" s="1">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
-        <v>2</v>
+      <c r="C19" s="1">
+        <v>0</v>
       </c>
       <c r="D19" s="1">
         <v>0</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>14</v>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -689,11 +717,11 @@
       <c r="D20" s="1">
         <v>0</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>14</v>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -709,11 +737,11 @@
       <c r="D21" s="1">
         <v>0</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>14</v>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -729,11 +757,11 @@
       <c r="D22" s="1">
         <v>0</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>14</v>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -749,11 +777,11 @@
       <c r="D23" s="1">
         <v>0</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>14</v>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -791,11 +819,11 @@
       <c r="D27" s="1">
         <v>0</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>14</v>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -805,17 +833,17 @@
       <c r="B28" s="1">
         <v>0</v>
       </c>
-      <c r="C28" s="3">
-        <v>2</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>14</v>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -831,11 +859,11 @@
       <c r="D29" s="1">
         <v>0</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>14</v>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -845,17 +873,17 @@
       <c r="B30" s="1">
         <v>0</v>
       </c>
-      <c r="C30" s="3">
-        <v>2</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>14</v>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -871,16 +899,16 @@
       <c r="D31" s="1">
         <v>0</v>
       </c>
-      <c r="E31" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>14</v>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="C33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -904,14 +932,20 @@
       <c r="A35" t="s">
         <v>8</v>
       </c>
-      <c r="B35">
-        <v>0</v>
+      <c r="B35" s="3">
+        <v>3</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35" s="4">
-        <v>1.5</v>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" s="1">
+        <v>0</v>
+      </c>
+      <c r="F35" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -924,36 +958,54 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36" s="4">
-        <v>1.5</v>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>10</v>
       </c>
-      <c r="B37">
-        <v>0</v>
+      <c r="B37" s="3">
+        <v>3</v>
       </c>
       <c r="C37">
         <v>0</v>
       </c>
-      <c r="D37" s="4">
-        <v>1.5</v>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>0</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>11</v>
       </c>
-      <c r="B38">
-        <v>0</v>
+      <c r="B38" s="3">
+        <v>3</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38" s="4">
-        <v>1.5</v>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>0</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -967,6 +1019,12 @@
         <v>0</v>
       </c>
       <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>0</v>
+      </c>
+      <c r="F39" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated R3 and Time_Worked
</commit_message>
<xml_diff>
--- a/Reports/Time_Worked.xlsx
+++ b/Reports/Time_Worked.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="15">
   <si>
     <t>Documentation</t>
   </si>
@@ -54,13 +54,13 @@
     <t>Calle</t>
   </si>
   <si>
-    <t>Andreas</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>UML</t>
+  </si>
+  <si>
+    <t>Research</t>
   </si>
 </sst>
 </file>
@@ -405,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F39"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -420,7 +420,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -450,11 +450,11 @@
       <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
+      <c r="D3" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E3" s="2">
+        <v>5.0999999999999996</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -470,11 +470,11 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
+      <c r="D4" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="E4" s="2">
+        <v>4.5999999999999996</v>
       </c>
       <c r="F4" s="1">
         <v>0</v>
@@ -490,11 +490,11 @@
       <c r="C5" s="1">
         <v>0</v>
       </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
+      <c r="D5" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="E5" s="2">
+        <v>6.1</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -510,35 +510,22 @@
       <c r="C6" s="1">
         <v>0</v>
       </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
+      <c r="D6" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>5.0999999999999996</v>
       </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="C9" t="s">
@@ -572,11 +559,11 @@
       <c r="C11" s="1">
         <v>0</v>
       </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
+      <c r="D11" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>1.5</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -595,8 +582,8 @@
       <c r="D12" s="1">
         <v>0</v>
       </c>
-      <c r="E12" s="1">
-        <v>0</v>
+      <c r="E12" s="2">
+        <v>1</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -612,11 +599,11 @@
       <c r="C13" s="1">
         <v>0</v>
       </c>
-      <c r="D13" s="1">
-        <v>0</v>
-      </c>
-      <c r="E13" s="1">
-        <v>0</v>
+      <c r="D13" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E13" s="2">
+        <v>1.5</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -632,35 +619,21 @@
       <c r="C14" s="1">
         <v>0</v>
       </c>
-      <c r="D14" s="1">
-        <v>0</v>
-      </c>
-      <c r="E14" s="1">
-        <v>0</v>
+      <c r="D14" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.5</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="1">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="C17" t="s">
@@ -765,24 +738,11 @@
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="1">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
-        <v>0</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0</v>
-      </c>
-      <c r="E23" s="1">
-        <v>0</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0</v>
-      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
     </row>
     <row r="25" spans="1:6">
       <c r="C25" t="s">
@@ -887,28 +847,15 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="1">
-        <v>0</v>
-      </c>
-      <c r="C31" s="1">
-        <v>0</v>
-      </c>
-      <c r="D31" s="1">
-        <v>0</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0</v>
-      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
     </row>
     <row r="33" spans="1:6">
       <c r="C33" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -938,11 +885,11 @@
       <c r="C35">
         <v>0</v>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0</v>
+      <c r="D35" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E35" s="2">
+        <v>3.6</v>
       </c>
       <c r="F35" s="1">
         <v>0</v>
@@ -958,11 +905,11 @@
       <c r="C36">
         <v>0</v>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
+      <c r="D36" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3.6</v>
       </c>
       <c r="F36" s="1">
         <v>0</v>
@@ -978,11 +925,11 @@
       <c r="C37">
         <v>0</v>
       </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <v>0</v>
+      <c r="D37" s="3">
+        <v>3.6</v>
+      </c>
+      <c r="E37" s="2">
+        <v>3.6</v>
       </c>
       <c r="F37" s="1">
         <v>0</v>
@@ -998,33 +945,119 @@
       <c r="C38">
         <v>0</v>
       </c>
-      <c r="D38">
-        <v>0</v>
-      </c>
-      <c r="E38" s="1">
-        <v>0</v>
+      <c r="D38" s="3">
+        <v>2.6</v>
+      </c>
+      <c r="E38" s="2">
+        <v>3.6</v>
       </c>
       <c r="F38" s="1">
         <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" t="s">
-        <v>12</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-      <c r="C39">
-        <v>0</v>
-      </c>
-      <c r="D39">
-        <v>0</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1">
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="C41" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="1">
+        <v>0</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>0</v>
+      </c>
+      <c r="E43" s="1">
+        <v>0</v>
+      </c>
+      <c r="F43" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>9</v>
+      </c>
+      <c r="B44" s="1">
+        <v>0</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>0</v>
+      </c>
+      <c r="F44" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="1">
+        <v>0</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
+      <c r="F45" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1">
+        <v>0</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>0</v>
+      </c>
+      <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>